<commit_message>
Revise spreadsheet for test cases
</commit_message>
<xml_diff>
--- a/workstream1/test_cases/CMF_applications_checks.xlsx
+++ b/workstream1/test_cases/CMF_applications_checks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucf-my.sharepoint.com/personal/le279259_ucf_edu/Documents/Documents/Service/DataKind/Housing/affordable-housing-tooling/workstream1/test_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{6A1EE31C-57CB-4EA2-B07B-25C353010C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45C4341B-D10A-413F-B89A-D17D27D5338F}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{6A1EE31C-57CB-4EA2-B07B-25C353010C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D3F1569-03BC-49FB-8A56-BCC890095B86}"/>
   <bookViews>
-    <workbookView xWindow="4272" yWindow="960" windowWidth="16752" windowHeight="10860" xr2:uid="{5D89FE43-4651-44C1-AD6E-3171EDB8D27B}"/>
+    <workbookView xWindow="9480" yWindow="792" windowWidth="13512" windowHeight="10860" xr2:uid="{5D89FE43-4651-44C1-AD6E-3171EDB8D27B}"/>
   </bookViews>
   <sheets>
     <sheet name="Checks" sheetId="2" r:id="rId1"/>
@@ -319,8 +319,8 @@
   <numFmts count="4">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -623,7 +623,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="6" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -651,11 +651,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="7" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -665,67 +665,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -798,6 +738,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -813,6 +763,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1188,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{038C0DE1-25F2-4B48-B2EB-2B484AA7FBDF}">
   <dimension ref="A1:AN20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1240,19 +1200,19 @@
         <v>units_allocated</v>
       </c>
       <c r="C1" s="24" t="str">
-        <f>AI1</f>
+        <f t="shared" ref="C1:D3" si="0">AI1</f>
         <v>Percent of Units at 50% AMI or Below</v>
       </c>
       <c r="D1" s="24" t="str">
-        <f>AJ1</f>
+        <f t="shared" si="0"/>
         <v>Units in Targeted Areas</v>
       </c>
       <c r="E1" s="24" t="str">
-        <f>AM1</f>
+        <f t="shared" ref="E1:F3" si="1">AM1</f>
         <v>Multiplier</v>
       </c>
       <c r="F1" s="24" t="str">
-        <f>AN1</f>
+        <f t="shared" si="1"/>
         <v>Multiplier &gt; 10</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -1368,19 +1328,19 @@
         <v>bolUnitCheck</v>
       </c>
       <c r="C2" s="24" t="str">
-        <f>AI2</f>
+        <f t="shared" si="0"/>
         <v>txtPctUnitsUnder50</v>
       </c>
       <c r="D2" s="24" t="str">
-        <f>AJ2</f>
+        <f t="shared" si="0"/>
         <v>txtReturnUnits</v>
       </c>
       <c r="E2" s="27" t="str">
-        <f>AM2</f>
+        <f t="shared" si="1"/>
         <v>Multiplier</v>
       </c>
       <c r="F2" s="24" t="str">
-        <f>AN2</f>
+        <f t="shared" si="1"/>
         <v>mult_gt_lt_10</v>
       </c>
       <c r="G2" s="20" t="s">
@@ -1496,19 +1456,19 @@
         <v>check</v>
       </c>
       <c r="C3" s="26">
-        <f>AI3</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="D3" s="24">
-        <f>AJ3</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="E3" s="27">
-        <f>AM3</f>
+        <f t="shared" si="1"/>
         <v>20.100000000000001</v>
       </c>
       <c r="F3" s="24" t="str">
-        <f>AN3</f>
+        <f t="shared" si="1"/>
         <v>&gt; 10</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -1640,15 +1600,15 @@
         <v>0.25</v>
       </c>
       <c r="D4" s="24">
-        <f t="shared" ref="D4" si="0">AJ4</f>
+        <f t="shared" ref="D4" si="2">AJ4</f>
         <v>72</v>
       </c>
       <c r="E4" s="27">
-        <f t="shared" ref="E4" si="1">AM4</f>
+        <f t="shared" ref="E4" si="3">AM4</f>
         <v>20.100000000000001</v>
       </c>
       <c r="F4" s="24" t="str">
-        <f t="shared" ref="F4" si="2">AN4</f>
+        <f t="shared" ref="F4" si="4">AN4</f>
         <v>&gt; 10</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -1768,27 +1728,27 @@
     </row>
     <row r="5" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="str">
-        <f t="shared" ref="A5:A6" si="3">U5</f>
+        <f t="shared" ref="A5:A6" si="5">U5</f>
         <v>check</v>
       </c>
       <c r="B5" s="24" t="str">
-        <f t="shared" ref="B5:B6" si="4">AF5</f>
+        <f t="shared" ref="B5:B6" si="6">AF5</f>
         <v>check</v>
       </c>
       <c r="C5" s="26">
-        <f t="shared" ref="C5:C6" si="5">AI5</f>
+        <f t="shared" ref="C5:C6" si="7">AI5</f>
         <v>0.25</v>
       </c>
       <c r="D5" s="24">
-        <f t="shared" ref="D5:D6" si="6">AJ5</f>
+        <f t="shared" ref="D5:D6" si="8">AJ5</f>
         <v>72</v>
       </c>
       <c r="E5" s="27">
-        <f t="shared" ref="E5:E6" si="7">AM5</f>
+        <f t="shared" ref="E5:E6" si="9">AM5</f>
         <v>20.100000000000001</v>
       </c>
       <c r="F5" s="24" t="str">
-        <f t="shared" ref="F5:F6" si="8">AN5</f>
+        <f t="shared" ref="F5:F6" si="10">AN5</f>
         <v>&gt; 10</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -1834,15 +1794,15 @@
         <v>7647015</v>
       </c>
       <c r="U5" s="8" t="str">
-        <f t="shared" ref="U5:U6" si="9">IF(SUM(R5:T5)+X5=Q5, "check", "error")</f>
+        <f t="shared" ref="U5:U6" si="11">IF(SUM(R5:T5)+X5=Q5, "check", "error")</f>
         <v>check</v>
       </c>
       <c r="V5" s="15">
-        <f t="shared" ref="V5:V6" si="10">R5+S5</f>
+        <f t="shared" ref="V5:V6" si="12">R5+S5</f>
         <v>20100000</v>
       </c>
       <c r="W5" s="15">
-        <f t="shared" ref="W5:W6" si="11">T5</f>
+        <f t="shared" ref="W5:W6" si="13">T5</f>
         <v>7647015</v>
       </c>
       <c r="X5" s="6">
@@ -1870,65 +1830,65 @@
         <v>0</v>
       </c>
       <c r="AF5" s="9" t="str">
-        <f t="shared" ref="AF5:AF6" si="12">IF(SUM(Z5:AE5)=Y5, "check", "error")</f>
+        <f t="shared" ref="AF5:AF6" si="14">IF(SUM(Z5:AE5)=Y5, "check", "error")</f>
         <v>check</v>
       </c>
       <c r="AG5" s="16">
-        <f t="shared" ref="AG5:AG6" si="13">Y5</f>
+        <f t="shared" ref="AG5:AG6" si="15">Y5</f>
         <v>72</v>
       </c>
       <c r="AH5" s="16">
-        <f t="shared" ref="AH5:AH6" si="14">SUM(Z5:AA5)</f>
+        <f t="shared" ref="AH5:AH6" si="16">SUM(Z5:AA5)</f>
         <v>18</v>
       </c>
       <c r="AI5" s="25">
-        <f t="shared" ref="AI5:AI6" si="15">AH5/AG5</f>
+        <f t="shared" ref="AI5:AI6" si="17">AH5/AG5</f>
         <v>0.25</v>
       </c>
       <c r="AJ5" s="16">
-        <f t="shared" ref="AJ5:AJ6" si="16">IF(OR(O5="Y",P5="Y"),Y5,0)</f>
+        <f t="shared" ref="AJ5:AJ6" si="18">IF(OR(O5="Y",P5="Y"),Y5,0)</f>
         <v>72</v>
       </c>
       <c r="AK5" s="17">
-        <f t="shared" ref="AK5:AK6" si="17">X5</f>
+        <f t="shared" ref="AK5:AK6" si="19">X5</f>
         <v>1000000</v>
       </c>
       <c r="AL5" s="18">
-        <f t="shared" ref="AL5:AL6" si="18">V5</f>
+        <f t="shared" ref="AL5:AL6" si="20">V5</f>
         <v>20100000</v>
       </c>
       <c r="AM5" s="19">
-        <f t="shared" ref="AM5:AM6" si="19">ROUND(AL5/X5,2)</f>
+        <f t="shared" ref="AM5:AM6" si="21">ROUND(AL5/X5,2)</f>
         <v>20.100000000000001</v>
       </c>
       <c r="AN5" s="22" t="str">
-        <f t="shared" ref="AN5:AN6" si="20">IF(AM5&gt;10,"&gt; 10","&lt;= 10")</f>
+        <f t="shared" ref="AN5:AN6" si="22">IF(AM5&gt;10,"&gt; 10","&lt;= 10")</f>
         <v>&gt; 10</v>
       </c>
     </row>
     <row r="6" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>check</v>
       </c>
       <c r="B6" s="24" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>check</v>
       </c>
       <c r="C6" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.25</v>
       </c>
       <c r="D6" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E6" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>20.100000000000001</v>
       </c>
       <c r="F6" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>&gt; 10</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -1974,15 +1934,15 @@
         <v>7647015</v>
       </c>
       <c r="U6" s="8" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>check</v>
       </c>
       <c r="V6" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>20100000</v>
       </c>
       <c r="W6" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7647015</v>
       </c>
       <c r="X6" s="6">
@@ -2010,49 +1970,49 @@
         <v>0</v>
       </c>
       <c r="AF6" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>check</v>
       </c>
       <c r="AG6" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>72</v>
       </c>
       <c r="AH6" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>18</v>
       </c>
       <c r="AI6" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.25</v>
       </c>
       <c r="AJ6" s="16">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AK6" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1000000</v>
       </c>
       <c r="AL6" s="18">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>20100000</v>
       </c>
       <c r="AM6" s="19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>20.100000000000001</v>
       </c>
       <c r="AN6" s="22" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>&gt; 10</v>
       </c>
     </row>
     <row r="7" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="24" t="str">
-        <f t="shared" ref="A7:A20" si="21">U7</f>
+        <f t="shared" ref="A7:A20" si="23">U7</f>
         <v>check</v>
       </c>
       <c r="B7" s="24" t="str">
-        <f t="shared" ref="B7:B20" si="22">AF7</f>
+        <f t="shared" ref="B7:B20" si="24">AF7</f>
         <v>check</v>
       </c>
       <c r="C7" s="26">
@@ -2114,15 +2074,15 @@
         <v>0</v>
       </c>
       <c r="U7" s="8" t="str">
-        <f t="shared" ref="U7:U20" si="23">IF(SUM(R7:T7)+X7=Q7, "check", "error")</f>
+        <f t="shared" ref="U7:U20" si="25">IF(SUM(R7:T7)+X7=Q7, "check", "error")</f>
         <v>check</v>
       </c>
       <c r="V7" s="15">
-        <f t="shared" ref="V7:V20" si="24">R7+S7</f>
+        <f t="shared" ref="V7:V20" si="26">R7+S7</f>
         <v>11793632</v>
       </c>
       <c r="W7" s="15">
-        <f t="shared" ref="W7:W20" si="25">T7</f>
+        <f t="shared" ref="W7:W20" si="27">T7</f>
         <v>0</v>
       </c>
       <c r="X7" s="13">
@@ -2150,27 +2110,27 @@
         <v>0</v>
       </c>
       <c r="AF7" s="9" t="str">
-        <f t="shared" ref="AF7:AF20" si="26">IF(SUM(Z7:AE7)=Y7, "check", "error")</f>
+        <f t="shared" ref="AF7:AF20" si="28">IF(SUM(Z7:AE7)=Y7, "check", "error")</f>
         <v>check</v>
       </c>
       <c r="AG7" s="16">
-        <f t="shared" ref="AG7:AG20" si="27">Y7</f>
+        <f t="shared" ref="AG7:AG20" si="29">Y7</f>
         <v>40</v>
       </c>
       <c r="AH7" s="16">
-        <f t="shared" ref="AH7:AH20" si="28">SUM(Z7:AA7)</f>
+        <f t="shared" ref="AH7:AH20" si="30">SUM(Z7:AA7)</f>
         <v>40</v>
       </c>
       <c r="AI7" s="25">
-        <f t="shared" ref="AI7:AI20" si="29">AH7/AG7</f>
+        <f t="shared" ref="AI7:AI20" si="31">AH7/AG7</f>
         <v>1</v>
       </c>
       <c r="AJ7" s="16">
-        <f t="shared" ref="AJ7:AJ20" si="30">IF(OR(O7="Y",P7="Y"),Y7,0)</f>
+        <f t="shared" ref="AJ7:AJ20" si="32">IF(OR(O7="Y",P7="Y"),Y7,0)</f>
         <v>40</v>
       </c>
       <c r="AK7" s="17">
-        <f t="shared" ref="AK7:AK20" si="31">X7</f>
+        <f t="shared" ref="AK7:AK20" si="33">X7</f>
         <v>1000000</v>
       </c>
       <c r="AL7" s="18">
@@ -2182,33 +2142,33 @@
         <v>11.79</v>
       </c>
       <c r="AN7" s="22" t="str">
-        <f t="shared" ref="AN7:AN20" si="32">IF(AM7&gt;10,"&gt; 10","&lt;= 10")</f>
+        <f t="shared" ref="AN7:AN20" si="34">IF(AM7&gt;10,"&gt; 10","&lt;= 10")</f>
         <v>&gt; 10</v>
       </c>
     </row>
     <row r="8" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="24" t="str">
-        <f t="shared" ref="A8:A9" si="33">U8</f>
+        <f t="shared" ref="A8:A9" si="35">U8</f>
         <v>error</v>
       </c>
       <c r="B8" s="24" t="str">
-        <f t="shared" ref="B8:B9" si="34">AF8</f>
+        <f t="shared" ref="B8:B9" si="36">AF8</f>
         <v>check</v>
       </c>
       <c r="C8" s="26">
-        <f t="shared" ref="C8:C9" si="35">AI8</f>
+        <f t="shared" ref="C8:C9" si="37">AI8</f>
         <v>1</v>
       </c>
       <c r="D8" s="24">
-        <f t="shared" ref="D8:D9" si="36">AJ8</f>
+        <f t="shared" ref="D8:D9" si="38">AJ8</f>
         <v>40</v>
       </c>
       <c r="E8" s="27">
-        <f t="shared" ref="E8:E9" si="37">AM8</f>
+        <f t="shared" ref="E8:E9" si="39">AM8</f>
         <v>11.79</v>
       </c>
       <c r="F8" s="24" t="str">
-        <f t="shared" ref="F8:F9" si="38">AN8</f>
+        <f t="shared" ref="F8:F9" si="40">AN8</f>
         <v>&gt; 10</v>
       </c>
       <c r="G8" s="11" t="s">
@@ -2254,15 +2214,15 @@
         <v>0</v>
       </c>
       <c r="U8" s="8" t="str">
-        <f t="shared" ref="U8:U9" si="39">IF(SUM(R8:T8)+X8=Q8, "check", "error")</f>
+        <f t="shared" ref="U8:U9" si="41">IF(SUM(R8:T8)+X8=Q8, "check", "error")</f>
         <v>error</v>
       </c>
       <c r="V8" s="15">
-        <f t="shared" ref="V8:V9" si="40">R8+S8</f>
+        <f t="shared" ref="V8:V9" si="42">R8+S8</f>
         <v>11793632</v>
       </c>
       <c r="W8" s="15">
-        <f t="shared" ref="W8:W9" si="41">T8</f>
+        <f t="shared" ref="W8:W9" si="43">T8</f>
         <v>0</v>
       </c>
       <c r="X8" s="13">
@@ -2290,65 +2250,65 @@
         <v>0</v>
       </c>
       <c r="AF8" s="9" t="str">
-        <f t="shared" ref="AF8:AF9" si="42">IF(SUM(Z8:AE8)=Y8, "check", "error")</f>
+        <f t="shared" ref="AF8:AF9" si="44">IF(SUM(Z8:AE8)=Y8, "check", "error")</f>
         <v>check</v>
       </c>
       <c r="AG8" s="16">
-        <f t="shared" ref="AG8:AG9" si="43">Y8</f>
+        <f t="shared" ref="AG8:AG9" si="45">Y8</f>
         <v>40</v>
       </c>
       <c r="AH8" s="16">
-        <f t="shared" ref="AH8:AH9" si="44">SUM(Z8:AA8)</f>
+        <f t="shared" ref="AH8:AH9" si="46">SUM(Z8:AA8)</f>
         <v>40</v>
       </c>
       <c r="AI8" s="25">
-        <f t="shared" ref="AI8:AI9" si="45">AH8/AG8</f>
+        <f t="shared" ref="AI8:AI9" si="47">AH8/AG8</f>
         <v>1</v>
       </c>
       <c r="AJ8" s="16">
-        <f t="shared" ref="AJ8:AJ9" si="46">IF(OR(O8="Y",P8="Y"),Y8,0)</f>
+        <f t="shared" ref="AJ8:AJ9" si="48">IF(OR(O8="Y",P8="Y"),Y8,0)</f>
         <v>40</v>
       </c>
       <c r="AK8" s="17">
-        <f t="shared" ref="AK8:AK9" si="47">X8</f>
+        <f t="shared" ref="AK8:AK9" si="49">X8</f>
         <v>1000000</v>
       </c>
       <c r="AL8" s="18">
-        <f t="shared" ref="AL8:AL9" si="48">V8</f>
+        <f t="shared" ref="AL8:AL9" si="50">V8</f>
         <v>11793632</v>
       </c>
       <c r="AM8" s="19">
-        <f t="shared" ref="AM8:AM9" si="49">ROUND(AL8/X8,2)</f>
+        <f t="shared" ref="AM8:AM9" si="51">ROUND(AL8/X8,2)</f>
         <v>11.79</v>
       </c>
       <c r="AN8" s="22" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>&gt; 10</v>
       </c>
     </row>
     <row r="9" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="24" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>check</v>
       </c>
       <c r="B9" s="24" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>error</v>
       </c>
       <c r="C9" s="26">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.8</v>
       </c>
       <c r="D9" s="24">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>50</v>
       </c>
       <c r="E9" s="27">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>11.79</v>
       </c>
       <c r="F9" s="24" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>&gt; 10</v>
       </c>
       <c r="G9" s="11" t="s">
@@ -2394,15 +2354,15 @@
         <v>0</v>
       </c>
       <c r="U9" s="8" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>check</v>
       </c>
       <c r="V9" s="15">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>11793632</v>
       </c>
       <c r="W9" s="15">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="X9" s="13">
@@ -2430,65 +2390,65 @@
         <v>0</v>
       </c>
       <c r="AF9" s="9" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>error</v>
       </c>
       <c r="AG9" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>50</v>
       </c>
       <c r="AH9" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>40</v>
       </c>
       <c r="AI9" s="25">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0.8</v>
       </c>
       <c r="AJ9" s="16">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>50</v>
       </c>
       <c r="AK9" s="17">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>1000000</v>
       </c>
       <c r="AL9" s="18">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>11793632</v>
       </c>
       <c r="AM9" s="19">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>11.79</v>
       </c>
       <c r="AN9" s="22" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>&gt; 10</v>
       </c>
     </row>
     <row r="10" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>check</v>
       </c>
       <c r="B10" s="24" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>check</v>
       </c>
       <c r="C10" s="26">
-        <f>AI10</f>
+        <f t="shared" ref="C10:C20" si="52">AI10</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="D10" s="24">
-        <f>AJ10</f>
+        <f t="shared" ref="D10:D20" si="53">AJ10</f>
         <v>21</v>
       </c>
       <c r="E10" s="27">
-        <f>AM10</f>
+        <f t="shared" ref="E10:E20" si="54">AM10</f>
         <v>0</v>
       </c>
       <c r="F10" s="24" t="str">
-        <f>AN10</f>
+        <f t="shared" ref="F10:F20" si="55">AN10</f>
         <v>&lt;= 10</v>
       </c>
       <c r="G10" s="11" t="s">
@@ -2534,15 +2494,15 @@
         <v>521176</v>
       </c>
       <c r="U10" s="8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>check</v>
       </c>
       <c r="V10" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="W10" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>521176</v>
       </c>
       <c r="X10" s="13">
@@ -2570,65 +2530,65 @@
         <v>0</v>
       </c>
       <c r="AF10" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>check</v>
       </c>
       <c r="AG10" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>21</v>
       </c>
       <c r="AH10" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>14</v>
       </c>
       <c r="AI10" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="AJ10" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>21</v>
       </c>
       <c r="AK10" s="17">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>175000</v>
       </c>
       <c r="AL10" s="18">
-        <f>V10</f>
+        <f t="shared" ref="AL10:AL20" si="56">V10</f>
         <v>0</v>
       </c>
       <c r="AM10" s="19">
-        <f>ROUND(AL10/X10,2)</f>
+        <f t="shared" ref="AM10:AM20" si="57">ROUND(AL10/X10,2)</f>
         <v>0</v>
       </c>
       <c r="AN10" s="22" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>&lt;= 10</v>
       </c>
     </row>
     <row r="11" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>check</v>
       </c>
       <c r="B11" s="24" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>check</v>
       </c>
       <c r="C11" s="26">
-        <f>AI11</f>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="D11" s="24">
-        <f>AJ11</f>
+        <f t="shared" si="53"/>
         <v>28</v>
       </c>
       <c r="E11" s="27">
-        <f>AM11</f>
+        <f t="shared" si="54"/>
         <v>2.46</v>
       </c>
       <c r="F11" s="24" t="str">
-        <f>AN11</f>
+        <f t="shared" si="55"/>
         <v>&lt;= 10</v>
       </c>
       <c r="G11" s="11" t="s">
@@ -2674,15 +2634,15 @@
         <v>0</v>
       </c>
       <c r="U11" s="8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>check</v>
       </c>
       <c r="V11" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1990000</v>
       </c>
       <c r="W11" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="X11" s="13">
@@ -2710,65 +2670,65 @@
         <v>0</v>
       </c>
       <c r="AF11" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>check</v>
       </c>
       <c r="AG11" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>28</v>
       </c>
       <c r="AH11" s="16">
-        <f t="shared" si="28"/>
-        <v>28</v>
-      </c>
-      <c r="AI11" s="25">
-        <f t="shared" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="AJ11" s="16">
         <f t="shared" si="30"/>
         <v>28</v>
       </c>
+      <c r="AI11" s="25">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="AJ11" s="16">
+        <f t="shared" si="32"/>
+        <v>28</v>
+      </c>
       <c r="AK11" s="17">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>810000</v>
       </c>
       <c r="AL11" s="18">
-        <f>V11</f>
+        <f t="shared" si="56"/>
         <v>1990000</v>
       </c>
       <c r="AM11" s="19">
-        <f>ROUND(AL11/X11,2)</f>
+        <f t="shared" si="57"/>
         <v>2.46</v>
       </c>
       <c r="AN11" s="22" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>&lt;= 10</v>
       </c>
     </row>
     <row r="12" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>check</v>
       </c>
       <c r="B12" s="24" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>check</v>
       </c>
       <c r="C12" s="26">
-        <f>AI12</f>
+        <f t="shared" si="52"/>
         <v>0.46875</v>
       </c>
       <c r="D12" s="24">
-        <f>AJ12</f>
+        <f t="shared" si="53"/>
         <v>32</v>
       </c>
       <c r="E12" s="27">
-        <f>AM12</f>
+        <f t="shared" si="54"/>
         <v>2.68</v>
       </c>
       <c r="F12" s="24" t="str">
-        <f>AN12</f>
+        <f t="shared" si="55"/>
         <v>&lt;= 10</v>
       </c>
       <c r="G12" s="11" t="s">
@@ -2814,15 +2774,15 @@
         <v>3000000</v>
       </c>
       <c r="U12" s="8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>check</v>
       </c>
       <c r="V12" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1340534</v>
       </c>
       <c r="W12" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>3000000</v>
       </c>
       <c r="X12" s="13">
@@ -2850,65 +2810,65 @@
         <v>0</v>
       </c>
       <c r="AF12" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>check</v>
       </c>
       <c r="AG12" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>32</v>
       </c>
       <c r="AH12" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>15</v>
       </c>
       <c r="AI12" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.46875</v>
       </c>
       <c r="AJ12" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>32</v>
       </c>
       <c r="AK12" s="17">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>500000</v>
       </c>
       <c r="AL12" s="18">
-        <f>V12</f>
+        <f t="shared" si="56"/>
         <v>1340534</v>
       </c>
       <c r="AM12" s="19">
-        <f>ROUND(AL12/X12,2)</f>
+        <f t="shared" si="57"/>
         <v>2.68</v>
       </c>
       <c r="AN12" s="22" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>&lt;= 10</v>
       </c>
     </row>
     <row r="13" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>check</v>
       </c>
       <c r="B13" s="24" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>check</v>
       </c>
       <c r="C13" s="26">
-        <f>AI13</f>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="D13" s="24">
-        <f>AJ13</f>
+        <f t="shared" si="53"/>
         <v>20</v>
       </c>
       <c r="E13" s="27">
-        <f>AM13</f>
+        <f t="shared" si="54"/>
         <v>4.0199999999999996</v>
       </c>
       <c r="F13" s="24" t="str">
-        <f>AN13</f>
+        <f t="shared" si="55"/>
         <v>&lt;= 10</v>
       </c>
       <c r="G13" s="11" t="s">
@@ -2954,15 +2914,15 @@
         <v>6236585</v>
       </c>
       <c r="U13" s="8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>check</v>
       </c>
       <c r="V13" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1086464</v>
       </c>
       <c r="W13" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>6236585</v>
       </c>
       <c r="X13" s="13">
@@ -2990,65 +2950,65 @@
         <v>0</v>
       </c>
       <c r="AF13" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>check</v>
       </c>
       <c r="AG13" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>20</v>
       </c>
       <c r="AH13" s="16">
-        <f t="shared" si="28"/>
-        <v>20</v>
-      </c>
-      <c r="AI13" s="25">
-        <f t="shared" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="AJ13" s="16">
         <f t="shared" si="30"/>
         <v>20</v>
       </c>
+      <c r="AI13" s="25">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="16">
+        <f t="shared" si="32"/>
+        <v>20</v>
+      </c>
       <c r="AK13" s="17">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>270000</v>
       </c>
       <c r="AL13" s="18">
-        <f>V13</f>
+        <f t="shared" si="56"/>
         <v>1086464</v>
       </c>
       <c r="AM13" s="19">
-        <f>ROUND(AL13/X13,2)</f>
+        <f t="shared" si="57"/>
         <v>4.0199999999999996</v>
       </c>
       <c r="AN13" s="22" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>&lt;= 10</v>
       </c>
     </row>
     <row r="14" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>check</v>
       </c>
       <c r="B14" s="24" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>check</v>
       </c>
       <c r="C14" s="26">
-        <f>AI14</f>
+        <f t="shared" si="52"/>
         <v>0.8</v>
       </c>
       <c r="D14" s="24">
-        <f>AJ14</f>
+        <f t="shared" si="53"/>
         <v>80</v>
       </c>
       <c r="E14" s="27">
-        <f>AM14</f>
+        <f t="shared" si="54"/>
         <v>17.149999999999999</v>
       </c>
       <c r="F14" s="24" t="str">
-        <f>AN14</f>
+        <f t="shared" si="55"/>
         <v>&gt; 10</v>
       </c>
       <c r="G14" s="11" t="s">
@@ -3094,15 +3054,15 @@
         <v>9050000</v>
       </c>
       <c r="U14" s="8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>check</v>
       </c>
       <c r="V14" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>17150000</v>
       </c>
       <c r="W14" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>9050000</v>
       </c>
       <c r="X14" s="13">
@@ -3130,65 +3090,65 @@
         <v>0</v>
       </c>
       <c r="AF14" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>check</v>
       </c>
       <c r="AG14" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>80</v>
       </c>
       <c r="AH14" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>64</v>
       </c>
       <c r="AI14" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.8</v>
       </c>
       <c r="AJ14" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>80</v>
       </c>
       <c r="AK14" s="17">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1000000</v>
       </c>
       <c r="AL14" s="18">
-        <f>V14</f>
+        <f t="shared" si="56"/>
         <v>17150000</v>
       </c>
       <c r="AM14" s="19">
-        <f>ROUND(AL14/X14,2)</f>
+        <f t="shared" si="57"/>
         <v>17.149999999999999</v>
       </c>
       <c r="AN14" s="22" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>&gt; 10</v>
       </c>
     </row>
     <row r="15" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>check</v>
       </c>
       <c r="B15" s="24" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>check</v>
       </c>
       <c r="C15" s="26">
-        <f>AI15</f>
+        <f t="shared" si="52"/>
         <v>0.10377358490566038</v>
       </c>
       <c r="D15" s="24">
-        <f>AJ15</f>
+        <f t="shared" si="53"/>
         <v>106</v>
       </c>
       <c r="E15" s="27">
-        <f>AM15</f>
+        <f t="shared" si="54"/>
         <v>17.100000000000001</v>
       </c>
       <c r="F15" s="24" t="str">
-        <f>AN15</f>
+        <f t="shared" si="55"/>
         <v>&gt; 10</v>
       </c>
       <c r="G15" s="11" t="s">
@@ -3234,15 +3194,15 @@
         <v>0</v>
       </c>
       <c r="U15" s="8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>check</v>
       </c>
       <c r="V15" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>17100000</v>
       </c>
       <c r="W15" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="X15" s="13">
@@ -3270,65 +3230,65 @@
         <v>0</v>
       </c>
       <c r="AF15" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>check</v>
       </c>
       <c r="AG15" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>106</v>
       </c>
       <c r="AH15" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>11</v>
       </c>
       <c r="AI15" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.10377358490566038</v>
       </c>
       <c r="AJ15" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>106</v>
       </c>
       <c r="AK15" s="17">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1000000</v>
       </c>
       <c r="AL15" s="18">
-        <f>V15</f>
+        <f t="shared" si="56"/>
         <v>17100000</v>
       </c>
       <c r="AM15" s="19">
-        <f>ROUND(AL15/X15,2)</f>
+        <f t="shared" si="57"/>
         <v>17.100000000000001</v>
       </c>
       <c r="AN15" s="22" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>&gt; 10</v>
       </c>
     </row>
     <row r="16" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>check</v>
       </c>
       <c r="B16" s="24" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>check</v>
       </c>
       <c r="C16" s="26">
-        <f>AI16</f>
+        <f t="shared" si="52"/>
         <v>0.20512820512820512</v>
       </c>
       <c r="D16" s="24">
-        <f>AJ16</f>
+        <f t="shared" si="53"/>
         <v>39</v>
       </c>
       <c r="E16" s="27">
-        <f>AM16</f>
+        <f t="shared" si="54"/>
         <v>5.98</v>
       </c>
       <c r="F16" s="24" t="str">
-        <f>AN16</f>
+        <f t="shared" si="55"/>
         <v>&lt;= 10</v>
       </c>
       <c r="G16" s="11" t="s">
@@ -3374,15 +3334,15 @@
         <v>4998000</v>
       </c>
       <c r="U16" s="8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>check</v>
       </c>
       <c r="V16" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1792936</v>
       </c>
       <c r="W16" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>4998000</v>
       </c>
       <c r="X16" s="13">
@@ -3410,65 +3370,65 @@
         <v>0</v>
       </c>
       <c r="AF16" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>check</v>
       </c>
       <c r="AG16" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>39</v>
       </c>
       <c r="AH16" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>8</v>
       </c>
       <c r="AI16" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.20512820512820512</v>
       </c>
       <c r="AJ16" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>39</v>
       </c>
       <c r="AK16" s="17">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>300000</v>
       </c>
       <c r="AL16" s="18">
-        <f>V16</f>
+        <f t="shared" si="56"/>
         <v>1792936</v>
       </c>
       <c r="AM16" s="19">
-        <f>ROUND(AL16/X16,2)</f>
+        <f t="shared" si="57"/>
         <v>5.98</v>
       </c>
       <c r="AN16" s="22" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>&lt;= 10</v>
       </c>
     </row>
     <row r="17" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>check</v>
       </c>
       <c r="B17" s="24" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>check</v>
       </c>
       <c r="C17" s="26">
-        <f>AI17</f>
+        <f t="shared" si="52"/>
         <v>0.22916666666666666</v>
       </c>
       <c r="D17" s="24">
-        <f>AJ17</f>
+        <f t="shared" si="53"/>
         <v>96</v>
       </c>
       <c r="E17" s="27">
-        <f>AM17</f>
+        <f t="shared" si="54"/>
         <v>9</v>
       </c>
       <c r="F17" s="24" t="str">
-        <f>AN17</f>
+        <f t="shared" si="55"/>
         <v>&lt;= 10</v>
       </c>
       <c r="G17" s="11" t="s">
@@ -3514,15 +3474,15 @@
         <v>16224664</v>
       </c>
       <c r="U17" s="8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>check</v>
       </c>
       <c r="V17" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1104400</v>
       </c>
       <c r="W17" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>16224664</v>
       </c>
       <c r="X17" s="13">
@@ -3550,65 +3510,65 @@
         <v>0</v>
       </c>
       <c r="AF17" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>check</v>
       </c>
       <c r="AG17" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>96</v>
       </c>
       <c r="AH17" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>22</v>
       </c>
       <c r="AI17" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.22916666666666666</v>
       </c>
       <c r="AJ17" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>96</v>
       </c>
       <c r="AK17" s="17">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>122711</v>
       </c>
       <c r="AL17" s="18">
-        <f>V17</f>
+        <f t="shared" si="56"/>
         <v>1104400</v>
       </c>
       <c r="AM17" s="19">
-        <f>ROUND(AL17/X17,2)</f>
+        <f t="shared" si="57"/>
         <v>9</v>
       </c>
       <c r="AN17" s="22" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>&lt;= 10</v>
       </c>
     </row>
     <row r="18" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>check</v>
       </c>
       <c r="B18" s="24" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>error</v>
       </c>
       <c r="C18" s="26">
-        <f>AI18</f>
+        <f t="shared" si="52"/>
         <v>0.32666666666666666</v>
       </c>
       <c r="D18" s="24">
-        <f>AJ18</f>
+        <f t="shared" si="53"/>
         <v>150</v>
       </c>
       <c r="E18" s="27">
-        <f>AM18</f>
+        <f t="shared" si="54"/>
         <v>12.53</v>
       </c>
       <c r="F18" s="24" t="str">
-        <f>AN18</f>
+        <f t="shared" si="55"/>
         <v>&gt; 10</v>
       </c>
       <c r="G18" s="11" t="s">
@@ -3654,15 +3614,15 @@
         <v>4988800</v>
       </c>
       <c r="U18" s="8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>check</v>
       </c>
       <c r="V18" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>12530760</v>
       </c>
       <c r="W18" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>4988800</v>
       </c>
       <c r="X18" s="13">
@@ -3690,65 +3650,65 @@
         <v>0</v>
       </c>
       <c r="AF18" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>error</v>
       </c>
       <c r="AG18" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>150</v>
       </c>
       <c r="AH18" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>49</v>
       </c>
       <c r="AI18" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.32666666666666666</v>
       </c>
       <c r="AJ18" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>150</v>
       </c>
       <c r="AK18" s="17">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1000000</v>
       </c>
       <c r="AL18" s="18">
-        <f>V18</f>
+        <f t="shared" si="56"/>
         <v>12530760</v>
       </c>
       <c r="AM18" s="19">
-        <f>ROUND(AL18/X18,2)</f>
+        <f t="shared" si="57"/>
         <v>12.53</v>
       </c>
       <c r="AN18" s="22" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>&gt; 10</v>
       </c>
     </row>
     <row r="19" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>check</v>
       </c>
       <c r="B19" s="24" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>error</v>
       </c>
       <c r="C19" s="26">
-        <f>AI19</f>
+        <f t="shared" si="52"/>
         <v>0.3</v>
       </c>
       <c r="D19" s="24">
-        <f>AJ19</f>
+        <f t="shared" si="53"/>
         <v>150</v>
       </c>
       <c r="E19" s="27">
-        <f>AM19</f>
+        <f t="shared" si="54"/>
         <v>10.45</v>
       </c>
       <c r="F19" s="24" t="str">
-        <f>AN19</f>
+        <f t="shared" si="55"/>
         <v>&gt; 10</v>
       </c>
       <c r="G19" s="11" t="s">
@@ -3794,15 +3754,15 @@
         <v>4677000</v>
       </c>
       <c r="U19" s="8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>check</v>
       </c>
       <c r="V19" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>10445638</v>
       </c>
       <c r="W19" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>4677000</v>
       </c>
       <c r="X19" s="13">
@@ -3830,65 +3790,65 @@
         <v>0</v>
       </c>
       <c r="AF19" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>error</v>
       </c>
       <c r="AG19" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>150</v>
       </c>
       <c r="AH19" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>45</v>
       </c>
       <c r="AI19" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="AJ19" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>150</v>
       </c>
       <c r="AK19" s="17">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1000000</v>
       </c>
       <c r="AL19" s="18">
-        <f>V19</f>
+        <f t="shared" si="56"/>
         <v>10445638</v>
       </c>
       <c r="AM19" s="19">
-        <f>ROUND(AL19/X19,2)</f>
+        <f t="shared" si="57"/>
         <v>10.45</v>
       </c>
       <c r="AN19" s="22" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>&gt; 10</v>
       </c>
     </row>
     <row r="20" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>check</v>
       </c>
       <c r="B20" s="24" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>check</v>
       </c>
       <c r="C20" s="26">
-        <f>AI20</f>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="D20" s="24">
-        <f>AJ20</f>
+        <f t="shared" si="53"/>
         <v>28</v>
       </c>
       <c r="E20" s="27">
-        <f>AM20</f>
+        <f t="shared" si="54"/>
         <v>2.77</v>
       </c>
       <c r="F20" s="24" t="str">
-        <f>AN20</f>
+        <f t="shared" si="55"/>
         <v>&lt;= 10</v>
       </c>
       <c r="G20" s="11" t="s">
@@ -3934,15 +3894,15 @@
         <v>6553632</v>
       </c>
       <c r="U20" s="8" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>check</v>
       </c>
       <c r="V20" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>2770243</v>
       </c>
       <c r="W20" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>6553632</v>
       </c>
       <c r="X20" s="13">
@@ -3970,122 +3930,102 @@
         <v>0</v>
       </c>
       <c r="AF20" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>check</v>
       </c>
       <c r="AG20" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>28</v>
       </c>
       <c r="AH20" s="16">
-        <f t="shared" si="28"/>
-        <v>28</v>
-      </c>
-      <c r="AI20" s="25">
-        <f t="shared" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="AJ20" s="16">
         <f t="shared" si="30"/>
         <v>28</v>
       </c>
+      <c r="AI20" s="25">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="AJ20" s="16">
+        <f t="shared" si="32"/>
+        <v>28</v>
+      </c>
       <c r="AK20" s="17">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1000000</v>
       </c>
       <c r="AL20" s="18">
-        <f>V20</f>
+        <f t="shared" si="56"/>
         <v>2770243</v>
       </c>
       <c r="AM20" s="19">
-        <f>ROUND(AL20/X20,2)</f>
+        <f t="shared" si="57"/>
         <v>2.77</v>
       </c>
       <c r="AN20" s="22" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>&lt;= 10</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:A20">
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+  <conditionalFormatting sqref="A3:B20">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+      <formula>"check"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
       <formula>"error"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
-      <formula>"check"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B20">
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>"error"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C20">
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="lessThan">
       <formula>0.45</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="greaterThan">
       <formula>0.45</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B20">
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
-      <formula>"check"</formula>
+  <conditionalFormatting sqref="D3:D20">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+      <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
-      <formula>"error"</formula>
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThan">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A20">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
-      <formula>"check"</formula>
+  <conditionalFormatting sqref="E3:E20">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
+      <formula>10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
-      <formula>"error"</formula>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
+      <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F20">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+      <formula>"&gt; 10"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"&lt;= 10"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"&lt;= 10"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"&gt; 10"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
       <formula>"""&gt; 10"""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="10" operator="equal">
       <formula>"""&lt;= 10"""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="equal">
       <formula>"""&lt;= 10"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E20">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="lessThan">
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThan">
-      <formula>10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D20">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F20">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"&gt; 10"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"&lt;= 10"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>